<commit_message>
NIH lagt i graphpa
</commit_message>
<xml_diff>
--- a/data_output/output for F24 stiff 2018-02-21 new CSA/reorg Youngs modulus alternative for Prism.xlsx
+++ b/data_output/output for F24 stiff 2018-02-21 new CSA/reorg Youngs modulus alternative for Prism.xlsx
@@ -9,10 +9,11 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9408"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9408" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Ark1" sheetId="1" r:id="rId1"/>
+    <sheet name="orig" sheetId="1" r:id="rId1"/>
+    <sheet name="PRISM" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="516" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="536" uniqueCount="18">
   <si>
     <t>Subject</t>
   </si>
@@ -67,13 +68,26 @@
   <si>
     <t>YM SOL common F cutoff</t>
   </si>
+  <si>
+    <t>con</t>
+  </si>
+  <si>
+    <t>str</t>
+  </si>
+  <si>
+    <t>pre</t>
+  </si>
+  <si>
+    <t>post</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="0.0E+00"/>
+    <numFmt numFmtId="166" formatCode="0.000E+00"/>
   </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
@@ -145,7 +159,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -162,6 +176,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="2" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="166" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="166" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -444,7 +462,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N89"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView topLeftCell="A55" workbookViewId="0">
       <selection activeCell="H1" sqref="H1"/>
     </sheetView>
   </sheetViews>
@@ -3753,4 +3771,1728 @@
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B1:AT27"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A26" sqref="A26"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="2" width="6.77734375" customWidth="1"/>
+    <col min="3" max="48" width="9.5546875" customWidth="1"/>
+    <col min="49" max="68" width="6.77734375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:46" x14ac:dyDescent="0.3">
+      <c r="B1" s="12" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="2:46" x14ac:dyDescent="0.3">
+      <c r="B2" s="13"/>
+      <c r="C2" t="s">
+        <v>16</v>
+      </c>
+      <c r="Y2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="3" spans="2:46" x14ac:dyDescent="0.3">
+      <c r="B3" s="13"/>
+      <c r="C3" s="2">
+        <v>1</v>
+      </c>
+      <c r="D3" s="2">
+        <v>3</v>
+      </c>
+      <c r="E3" s="2">
+        <v>4</v>
+      </c>
+      <c r="F3" s="3">
+        <v>6</v>
+      </c>
+      <c r="G3" s="2">
+        <v>7</v>
+      </c>
+      <c r="H3" s="2">
+        <v>8</v>
+      </c>
+      <c r="I3" s="2">
+        <v>9</v>
+      </c>
+      <c r="J3" s="3">
+        <v>10</v>
+      </c>
+      <c r="K3" s="2">
+        <v>11</v>
+      </c>
+      <c r="L3" s="2">
+        <v>16</v>
+      </c>
+      <c r="M3" s="2">
+        <v>18</v>
+      </c>
+      <c r="N3" s="3">
+        <v>19</v>
+      </c>
+      <c r="O3" s="2">
+        <v>20</v>
+      </c>
+      <c r="P3" s="2">
+        <v>21</v>
+      </c>
+      <c r="Q3" s="2">
+        <v>22</v>
+      </c>
+      <c r="R3" s="3">
+        <v>24</v>
+      </c>
+      <c r="S3" s="2">
+        <v>25</v>
+      </c>
+      <c r="T3" s="2">
+        <v>26</v>
+      </c>
+      <c r="U3" s="2">
+        <v>28</v>
+      </c>
+      <c r="V3" s="3">
+        <v>29</v>
+      </c>
+      <c r="W3" s="2">
+        <v>30</v>
+      </c>
+      <c r="X3" s="2">
+        <v>31</v>
+      </c>
+      <c r="Y3" s="2">
+        <v>1</v>
+      </c>
+      <c r="Z3" s="2">
+        <v>3</v>
+      </c>
+      <c r="AA3" s="2">
+        <v>4</v>
+      </c>
+      <c r="AB3" s="3">
+        <v>6</v>
+      </c>
+      <c r="AC3" s="2">
+        <v>7</v>
+      </c>
+      <c r="AD3" s="2">
+        <v>8</v>
+      </c>
+      <c r="AE3" s="2">
+        <v>9</v>
+      </c>
+      <c r="AF3" s="3">
+        <v>10</v>
+      </c>
+      <c r="AG3" s="2">
+        <v>11</v>
+      </c>
+      <c r="AH3" s="2">
+        <v>16</v>
+      </c>
+      <c r="AI3" s="2">
+        <v>18</v>
+      </c>
+      <c r="AJ3" s="3">
+        <v>19</v>
+      </c>
+      <c r="AK3" s="2">
+        <v>20</v>
+      </c>
+      <c r="AL3" s="2">
+        <v>21</v>
+      </c>
+      <c r="AM3" s="2">
+        <v>22</v>
+      </c>
+      <c r="AN3" s="3">
+        <v>24</v>
+      </c>
+      <c r="AO3" s="2">
+        <v>25</v>
+      </c>
+      <c r="AP3" s="2">
+        <v>26</v>
+      </c>
+      <c r="AQ3" s="2">
+        <v>28</v>
+      </c>
+      <c r="AR3" s="3">
+        <v>29</v>
+      </c>
+      <c r="AS3" s="2">
+        <v>30</v>
+      </c>
+      <c r="AT3" s="2">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="4" spans="2:46" x14ac:dyDescent="0.3">
+      <c r="B4" s="13" t="s">
+        <v>14</v>
+      </c>
+      <c r="C4" s="14">
+        <v>851969548.14074254</v>
+      </c>
+      <c r="D4" s="14">
+        <v>1270859798.8503022</v>
+      </c>
+      <c r="E4" s="14">
+        <v>1305832576.755682</v>
+      </c>
+      <c r="F4" s="14">
+        <v>754767948.5008626</v>
+      </c>
+      <c r="G4" s="14">
+        <v>1123739410.1358547</v>
+      </c>
+      <c r="H4" s="14">
+        <v>992760843.66540885</v>
+      </c>
+      <c r="I4" s="14">
+        <v>718794684.368011</v>
+      </c>
+      <c r="J4" s="14">
+        <v>961059307.26622033</v>
+      </c>
+      <c r="K4" s="14">
+        <v>515839974.69766283</v>
+      </c>
+      <c r="L4" s="14">
+        <v>1022999442.3420769</v>
+      </c>
+      <c r="M4" s="14">
+        <v>651303634.08263004</v>
+      </c>
+      <c r="N4" s="14">
+        <v>1107676417.8682346</v>
+      </c>
+      <c r="O4" s="14">
+        <v>1178941395.7798312</v>
+      </c>
+      <c r="P4" s="14">
+        <v>626475612.1977818</v>
+      </c>
+      <c r="Q4" s="14">
+        <v>1115292727.542269</v>
+      </c>
+      <c r="R4" s="14">
+        <v>1000040248.9511139</v>
+      </c>
+      <c r="S4" s="14">
+        <v>860001843.78625023</v>
+      </c>
+      <c r="T4" s="14">
+        <v>1310640855.9213998</v>
+      </c>
+      <c r="U4" s="14">
+        <v>902632359.76647961</v>
+      </c>
+      <c r="V4" s="14">
+        <v>1028917746.6752512</v>
+      </c>
+      <c r="W4" s="14">
+        <v>1201299355.6650245</v>
+      </c>
+      <c r="X4" s="14">
+        <v>1179500868.0228038</v>
+      </c>
+      <c r="Y4" s="14">
+        <v>842114459.20035923</v>
+      </c>
+      <c r="Z4" s="14">
+        <v>1466964398.8829432</v>
+      </c>
+      <c r="AA4" s="14">
+        <v>980281721.28601313</v>
+      </c>
+      <c r="AB4" s="14">
+        <v>752786704.17126966</v>
+      </c>
+      <c r="AC4" s="14">
+        <v>806092215.65421116</v>
+      </c>
+      <c r="AD4" s="14">
+        <v>716660289.33247852</v>
+      </c>
+      <c r="AE4" s="14">
+        <v>807340238.15230906</v>
+      </c>
+      <c r="AF4" s="14">
+        <v>1089641648.4831541</v>
+      </c>
+      <c r="AG4" s="14">
+        <v>1007809741.9814235</v>
+      </c>
+      <c r="AH4" s="14">
+        <v>1032319845.8373131</v>
+      </c>
+      <c r="AI4" s="14">
+        <v>757302214.99523866</v>
+      </c>
+      <c r="AJ4" s="14">
+        <v>938920971.5511719</v>
+      </c>
+      <c r="AK4" s="14">
+        <v>1160276761.5789061</v>
+      </c>
+      <c r="AL4" s="14">
+        <v>620045755.07680368</v>
+      </c>
+      <c r="AM4" s="14">
+        <v>890572502.63383222</v>
+      </c>
+      <c r="AN4" s="14">
+        <v>1105571180.5355871</v>
+      </c>
+      <c r="AO4" s="14">
+        <v>1302207522.1764858</v>
+      </c>
+      <c r="AP4" s="14">
+        <v>1162978231.7880616</v>
+      </c>
+      <c r="AQ4" s="14">
+        <v>680172455.34286261</v>
+      </c>
+      <c r="AR4" s="14">
+        <v>598631520.87029529</v>
+      </c>
+      <c r="AS4" s="14">
+        <v>1034443493.5210446</v>
+      </c>
+      <c r="AT4" s="14">
+        <v>824661985.86621082</v>
+      </c>
+    </row>
+    <row r="5" spans="2:46" x14ac:dyDescent="0.3">
+      <c r="B5" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="C5" s="14">
+        <v>522980874.45243704</v>
+      </c>
+      <c r="D5" s="14">
+        <v>1261555030.1216018</v>
+      </c>
+      <c r="E5" s="14">
+        <v>1177018615.1498401</v>
+      </c>
+      <c r="F5" s="14">
+        <v>895412416.1885972</v>
+      </c>
+      <c r="G5" s="14">
+        <v>919824945.32491338</v>
+      </c>
+      <c r="H5" s="14">
+        <v>870453666.32274127</v>
+      </c>
+      <c r="I5" s="14">
+        <v>624624696.39654493</v>
+      </c>
+      <c r="J5" s="14">
+        <v>922665826.07318318</v>
+      </c>
+      <c r="K5" s="14">
+        <v>739531213.40340567</v>
+      </c>
+      <c r="L5" s="14">
+        <v>990080047.98280883</v>
+      </c>
+      <c r="M5" s="14">
+        <v>1276314639.7500782</v>
+      </c>
+      <c r="N5" s="14">
+        <v>940137334.88636887</v>
+      </c>
+      <c r="O5" s="14">
+        <v>1284132523.5665221</v>
+      </c>
+      <c r="P5" s="14">
+        <v>831644920.63193893</v>
+      </c>
+      <c r="Q5" s="14">
+        <v>833120217.26439178</v>
+      </c>
+      <c r="R5" s="14">
+        <v>701156151.94670308</v>
+      </c>
+      <c r="S5" s="14">
+        <v>851616749.46335375</v>
+      </c>
+      <c r="T5" s="14">
+        <v>1225463842.5595841</v>
+      </c>
+      <c r="U5" s="14">
+        <v>959545858.8025111</v>
+      </c>
+      <c r="V5" s="14">
+        <v>697777878.77095366</v>
+      </c>
+      <c r="W5" s="14">
+        <v>882907415.26357555</v>
+      </c>
+      <c r="X5" s="14">
+        <v>1197667133.9320178</v>
+      </c>
+      <c r="Y5" s="14">
+        <v>692439195.52215397</v>
+      </c>
+      <c r="Z5" s="14">
+        <v>980669431.38368022</v>
+      </c>
+      <c r="AA5" s="14">
+        <v>765234119.01335382</v>
+      </c>
+      <c r="AB5" s="14">
+        <v>680879589.30593169</v>
+      </c>
+      <c r="AC5" s="14">
+        <v>851864294.31538224</v>
+      </c>
+      <c r="AD5" s="14">
+        <v>608679680.48692799</v>
+      </c>
+      <c r="AE5" s="14">
+        <v>621243644.92671788</v>
+      </c>
+      <c r="AF5" s="14">
+        <v>1040865420.646685</v>
+      </c>
+      <c r="AG5" s="14">
+        <v>552188800.81201172</v>
+      </c>
+      <c r="AH5" s="14">
+        <v>1104619869.5648143</v>
+      </c>
+      <c r="AI5" s="14">
+        <v>1056019280.6307224</v>
+      </c>
+      <c r="AJ5" s="15">
+        <v>501160974.76123124</v>
+      </c>
+      <c r="AK5" s="14">
+        <v>871196313.67342424</v>
+      </c>
+      <c r="AL5" s="14">
+        <v>493835127.061216</v>
+      </c>
+      <c r="AM5" s="14">
+        <v>1179316762.0523305</v>
+      </c>
+      <c r="AN5" s="14">
+        <v>726738654.07457364</v>
+      </c>
+      <c r="AO5" s="14">
+        <v>1042226732.2821054</v>
+      </c>
+      <c r="AP5" s="14">
+        <v>749754254.48478293</v>
+      </c>
+      <c r="AQ5" s="14">
+        <v>1018170502.7702712</v>
+      </c>
+      <c r="AR5" s="14">
+        <v>692698106.54181266</v>
+      </c>
+      <c r="AS5" s="14">
+        <v>982879641.96552396</v>
+      </c>
+      <c r="AT5" s="14">
+        <v>952169441.55222058</v>
+      </c>
+    </row>
+    <row r="6" spans="2:46" x14ac:dyDescent="0.3">
+      <c r="B6" s="13"/>
+    </row>
+    <row r="7" spans="2:46" x14ac:dyDescent="0.3">
+      <c r="B7" s="13"/>
+    </row>
+    <row r="8" spans="2:46" x14ac:dyDescent="0.3">
+      <c r="B8" s="12" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="9" spans="2:46" x14ac:dyDescent="0.3">
+      <c r="B9" s="13"/>
+      <c r="C9" t="s">
+        <v>16</v>
+      </c>
+      <c r="Y9" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="10" spans="2:46" x14ac:dyDescent="0.3">
+      <c r="B10" s="13"/>
+      <c r="C10" s="2">
+        <v>1</v>
+      </c>
+      <c r="D10" s="2">
+        <v>3</v>
+      </c>
+      <c r="E10" s="2">
+        <v>4</v>
+      </c>
+      <c r="F10" s="3">
+        <v>6</v>
+      </c>
+      <c r="G10" s="2">
+        <v>7</v>
+      </c>
+      <c r="H10" s="2">
+        <v>8</v>
+      </c>
+      <c r="I10" s="2">
+        <v>9</v>
+      </c>
+      <c r="J10" s="3">
+        <v>10</v>
+      </c>
+      <c r="K10" s="2">
+        <v>11</v>
+      </c>
+      <c r="L10" s="2">
+        <v>16</v>
+      </c>
+      <c r="M10" s="2">
+        <v>18</v>
+      </c>
+      <c r="N10" s="3">
+        <v>19</v>
+      </c>
+      <c r="O10" s="2">
+        <v>20</v>
+      </c>
+      <c r="P10" s="2">
+        <v>21</v>
+      </c>
+      <c r="Q10" s="2">
+        <v>22</v>
+      </c>
+      <c r="R10" s="3">
+        <v>24</v>
+      </c>
+      <c r="S10" s="2">
+        <v>25</v>
+      </c>
+      <c r="T10" s="2">
+        <v>26</v>
+      </c>
+      <c r="U10" s="2">
+        <v>28</v>
+      </c>
+      <c r="V10" s="3">
+        <v>29</v>
+      </c>
+      <c r="W10" s="2">
+        <v>30</v>
+      </c>
+      <c r="X10" s="2">
+        <v>31</v>
+      </c>
+      <c r="Y10" s="2">
+        <v>1</v>
+      </c>
+      <c r="Z10" s="2">
+        <v>3</v>
+      </c>
+      <c r="AA10" s="2">
+        <v>4</v>
+      </c>
+      <c r="AB10" s="3">
+        <v>6</v>
+      </c>
+      <c r="AC10" s="2">
+        <v>7</v>
+      </c>
+      <c r="AD10" s="2">
+        <v>8</v>
+      </c>
+      <c r="AE10" s="2">
+        <v>9</v>
+      </c>
+      <c r="AF10" s="3">
+        <v>10</v>
+      </c>
+      <c r="AG10" s="2">
+        <v>11</v>
+      </c>
+      <c r="AH10" s="2">
+        <v>16</v>
+      </c>
+      <c r="AI10" s="2">
+        <v>18</v>
+      </c>
+      <c r="AJ10" s="3">
+        <v>19</v>
+      </c>
+      <c r="AK10" s="2">
+        <v>20</v>
+      </c>
+      <c r="AL10" s="2">
+        <v>21</v>
+      </c>
+      <c r="AM10" s="2">
+        <v>22</v>
+      </c>
+      <c r="AN10" s="3">
+        <v>24</v>
+      </c>
+      <c r="AO10" s="2">
+        <v>25</v>
+      </c>
+      <c r="AP10" s="2">
+        <v>26</v>
+      </c>
+      <c r="AQ10" s="2">
+        <v>28</v>
+      </c>
+      <c r="AR10" s="3">
+        <v>29</v>
+      </c>
+      <c r="AS10" s="2">
+        <v>30</v>
+      </c>
+      <c r="AT10" s="2">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="11" spans="2:46" x14ac:dyDescent="0.3">
+      <c r="B11" s="13" t="s">
+        <v>14</v>
+      </c>
+      <c r="C11" s="14">
+        <v>869315466.85517001</v>
+      </c>
+      <c r="D11" s="14">
+        <v>1308240272.7069728</v>
+      </c>
+      <c r="E11" s="14">
+        <v>1338465476.6694517</v>
+      </c>
+      <c r="F11" s="14">
+        <v>768101398.47437692</v>
+      </c>
+      <c r="G11" s="14">
+        <v>1153274548.1190195</v>
+      </c>
+      <c r="H11" s="14">
+        <v>1015513392.2688731</v>
+      </c>
+      <c r="I11" s="14">
+        <v>739828792.71678269</v>
+      </c>
+      <c r="J11" s="14">
+        <v>987423948.99396324</v>
+      </c>
+      <c r="K11" s="14">
+        <v>526565242.2223981</v>
+      </c>
+      <c r="L11" s="14">
+        <v>1052082852.2632948</v>
+      </c>
+      <c r="M11" s="14">
+        <v>661110456.71611047</v>
+      </c>
+      <c r="N11" s="14">
+        <v>1139843834.5422881</v>
+      </c>
+      <c r="O11" s="14">
+        <v>1212330158.7272458</v>
+      </c>
+      <c r="P11" s="14">
+        <v>634040796.83882654</v>
+      </c>
+      <c r="Q11" s="14">
+        <v>1137745410.1008716</v>
+      </c>
+      <c r="R11" s="14">
+        <v>1027378706.1663963</v>
+      </c>
+      <c r="S11" s="14">
+        <v>881538016.20028973</v>
+      </c>
+      <c r="T11" s="14">
+        <v>1342134438.3588305</v>
+      </c>
+      <c r="U11" s="14">
+        <v>927602839.15179074</v>
+      </c>
+      <c r="V11" s="14">
+        <v>1054353452.5169834</v>
+      </c>
+      <c r="W11" s="14">
+        <v>1236425928.3356347</v>
+      </c>
+      <c r="X11" s="14">
+        <v>1213978908.1470528</v>
+      </c>
+      <c r="Y11" s="14">
+        <v>866579359.44814885</v>
+      </c>
+      <c r="Z11" s="14">
+        <v>1508902078.556519</v>
+      </c>
+      <c r="AA11" s="14">
+        <v>1006527743.9898821</v>
+      </c>
+      <c r="AB11" s="14">
+        <v>770375047.33078825</v>
+      </c>
+      <c r="AC11" s="14">
+        <v>828621121.57863033</v>
+      </c>
+      <c r="AD11" s="14">
+        <v>736696401.7747184</v>
+      </c>
+      <c r="AE11" s="14">
+        <v>828277112.98423922</v>
+      </c>
+      <c r="AF11" s="14">
+        <v>1120730057.2805338</v>
+      </c>
+      <c r="AG11" s="14">
+        <v>1036960118.0996168</v>
+      </c>
+      <c r="AH11" s="14">
+        <v>1060012620.8379647</v>
+      </c>
+      <c r="AI11" s="14">
+        <v>772779911.39825249</v>
+      </c>
+      <c r="AJ11" s="14">
+        <v>965860789.5426774</v>
+      </c>
+      <c r="AK11" s="14">
+        <v>1183342800.824841</v>
+      </c>
+      <c r="AL11" s="14">
+        <v>630962245.55259371</v>
+      </c>
+      <c r="AM11" s="14">
+        <v>906035252.47508526</v>
+      </c>
+      <c r="AN11" s="14">
+        <v>1138200151.3643453</v>
+      </c>
+      <c r="AO11" s="14">
+        <v>1339766772.903631</v>
+      </c>
+      <c r="AP11" s="14">
+        <v>1192184533.3024809</v>
+      </c>
+      <c r="AQ11" s="14">
+        <v>694576420.08147573</v>
+      </c>
+      <c r="AR11" s="14">
+        <v>611211186.31193233</v>
+      </c>
+      <c r="AS11" s="14">
+        <v>1064228543.3631331</v>
+      </c>
+      <c r="AT11" s="14">
+        <v>846830378.30618274</v>
+      </c>
+    </row>
+    <row r="12" spans="2:46" x14ac:dyDescent="0.3">
+      <c r="B12" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="C12" s="14">
+        <v>525361360.7266801</v>
+      </c>
+      <c r="D12" s="14">
+        <v>1298814977.7142947</v>
+      </c>
+      <c r="E12" s="14">
+        <v>1207083450.2605863</v>
+      </c>
+      <c r="F12" s="14">
+        <v>900700176.09133172</v>
+      </c>
+      <c r="G12" s="14">
+        <v>940027233.83886242</v>
+      </c>
+      <c r="H12" s="14">
+        <v>893576718.18990493</v>
+      </c>
+      <c r="I12" s="14">
+        <v>642442363.96972537</v>
+      </c>
+      <c r="J12" s="14">
+        <v>948995738.25093389</v>
+      </c>
+      <c r="K12" s="14">
+        <v>759228470.32231259</v>
+      </c>
+      <c r="L12" s="14">
+        <v>1017193250.7641392</v>
+      </c>
+      <c r="M12" s="14">
+        <v>1305180605.2990646</v>
+      </c>
+      <c r="N12" s="14">
+        <v>967940719.84589088</v>
+      </c>
+      <c r="O12" s="14">
+        <v>1322397453.9934211</v>
+      </c>
+      <c r="P12" s="14">
+        <v>844304720.33851445</v>
+      </c>
+      <c r="Q12" s="14">
+        <v>845469579.759197</v>
+      </c>
+      <c r="R12" s="14">
+        <v>720616472.07302153</v>
+      </c>
+      <c r="S12" s="14">
+        <v>870456848.58518887</v>
+      </c>
+      <c r="T12" s="14">
+        <v>1261207704.5671058</v>
+      </c>
+      <c r="U12" s="14">
+        <v>985341430.91032434</v>
+      </c>
+      <c r="V12" s="14">
+        <v>715943021.02372932</v>
+      </c>
+      <c r="W12" s="14">
+        <v>906832583.14170337</v>
+      </c>
+      <c r="X12" s="14">
+        <v>1232825574.9337699</v>
+      </c>
+      <c r="Y12" s="14">
+        <v>700174948.50500047</v>
+      </c>
+      <c r="Z12" s="14">
+        <v>1008241073.2561792</v>
+      </c>
+      <c r="AA12" s="14">
+        <v>784191714.96098995</v>
+      </c>
+      <c r="AB12" s="14">
+        <v>698064387.35369658</v>
+      </c>
+      <c r="AC12" s="14">
+        <v>875755718.45221937</v>
+      </c>
+      <c r="AD12" s="14">
+        <v>626308602.6533668</v>
+      </c>
+      <c r="AE12" s="14">
+        <v>638227729.7325561</v>
+      </c>
+      <c r="AF12" s="14">
+        <v>1071914252.6302229</v>
+      </c>
+      <c r="AG12" s="14">
+        <v>567834890.73812616</v>
+      </c>
+      <c r="AH12" s="14">
+        <v>1134820798.3913741</v>
+      </c>
+      <c r="AI12" s="14">
+        <v>1073716455.8515161</v>
+      </c>
+      <c r="AJ12" s="15">
+        <v>512263376.50275487</v>
+      </c>
+      <c r="AK12" s="14">
+        <v>896052117.13746059</v>
+      </c>
+      <c r="AL12" s="14">
+        <v>491571345.36967981</v>
+      </c>
+      <c r="AM12" s="14">
+        <v>1214411392.6190162</v>
+      </c>
+      <c r="AN12" s="14">
+        <v>746715214.59523988</v>
+      </c>
+      <c r="AO12" s="14">
+        <v>1071127577.3048053</v>
+      </c>
+      <c r="AP12" s="14">
+        <v>769687420.44450641</v>
+      </c>
+      <c r="AQ12" s="14">
+        <v>1048376276.0625254</v>
+      </c>
+      <c r="AR12" s="14">
+        <v>712880568.30299246</v>
+      </c>
+      <c r="AS12" s="14">
+        <v>1010754916.7823792</v>
+      </c>
+      <c r="AT12" s="14">
+        <v>978686288.63433492</v>
+      </c>
+    </row>
+    <row r="13" spans="2:46" x14ac:dyDescent="0.3">
+      <c r="B13" s="13"/>
+    </row>
+    <row r="14" spans="2:46" x14ac:dyDescent="0.3">
+      <c r="B14" s="13"/>
+    </row>
+    <row r="15" spans="2:46" x14ac:dyDescent="0.3">
+      <c r="B15" s="13"/>
+    </row>
+    <row r="16" spans="2:46" x14ac:dyDescent="0.3">
+      <c r="B16" s="12" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="17" spans="2:46" x14ac:dyDescent="0.3">
+      <c r="B17" s="13"/>
+      <c r="C17" t="s">
+        <v>16</v>
+      </c>
+      <c r="W17" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="18" spans="2:46" x14ac:dyDescent="0.3">
+      <c r="B18" s="13"/>
+      <c r="C18" s="2">
+        <v>1</v>
+      </c>
+      <c r="D18" s="2">
+        <v>3</v>
+      </c>
+      <c r="E18" s="2">
+        <v>4</v>
+      </c>
+      <c r="F18" s="3">
+        <v>6</v>
+      </c>
+      <c r="G18" s="2">
+        <v>7</v>
+      </c>
+      <c r="H18" s="2">
+        <v>8</v>
+      </c>
+      <c r="I18" s="2">
+        <v>9</v>
+      </c>
+      <c r="J18" s="3">
+        <v>10</v>
+      </c>
+      <c r="K18" s="2">
+        <v>11</v>
+      </c>
+      <c r="L18" s="2">
+        <v>13</v>
+      </c>
+      <c r="M18" s="2">
+        <v>15</v>
+      </c>
+      <c r="N18" s="3">
+        <v>16</v>
+      </c>
+      <c r="O18" s="2">
+        <v>18</v>
+      </c>
+      <c r="P18" s="2">
+        <v>20</v>
+      </c>
+      <c r="Q18" s="2">
+        <v>22</v>
+      </c>
+      <c r="R18" s="3">
+        <v>24</v>
+      </c>
+      <c r="S18" s="2">
+        <v>25</v>
+      </c>
+      <c r="T18" s="2">
+        <v>26</v>
+      </c>
+      <c r="U18" s="2">
+        <v>30</v>
+      </c>
+      <c r="V18" s="3">
+        <v>31</v>
+      </c>
+      <c r="W18" s="2">
+        <v>1</v>
+      </c>
+      <c r="X18" s="2">
+        <v>3</v>
+      </c>
+      <c r="Y18" s="2">
+        <v>4</v>
+      </c>
+      <c r="Z18" s="3">
+        <v>6</v>
+      </c>
+      <c r="AA18" s="2">
+        <v>7</v>
+      </c>
+      <c r="AB18" s="2">
+        <v>8</v>
+      </c>
+      <c r="AC18" s="2">
+        <v>9</v>
+      </c>
+      <c r="AD18" s="3">
+        <v>10</v>
+      </c>
+      <c r="AE18" s="2">
+        <v>11</v>
+      </c>
+      <c r="AF18" s="2">
+        <v>13</v>
+      </c>
+      <c r="AG18" s="2">
+        <v>15</v>
+      </c>
+      <c r="AH18" s="3">
+        <v>16</v>
+      </c>
+      <c r="AI18" s="2">
+        <v>18</v>
+      </c>
+      <c r="AJ18" s="2">
+        <v>20</v>
+      </c>
+      <c r="AK18" s="2">
+        <v>22</v>
+      </c>
+      <c r="AL18" s="3">
+        <v>24</v>
+      </c>
+      <c r="AM18" s="2">
+        <v>25</v>
+      </c>
+      <c r="AN18" s="2">
+        <v>26</v>
+      </c>
+      <c r="AO18" s="2">
+        <v>30</v>
+      </c>
+      <c r="AP18" s="3">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="19" spans="2:46" x14ac:dyDescent="0.3">
+      <c r="B19" s="13" t="s">
+        <v>14</v>
+      </c>
+      <c r="C19" s="14">
+        <v>737044958.29753768</v>
+      </c>
+      <c r="D19" s="14">
+        <v>522300989.15647358</v>
+      </c>
+      <c r="E19" s="14">
+        <v>331608136.32730883</v>
+      </c>
+      <c r="F19" s="14">
+        <v>294109328.90325809</v>
+      </c>
+      <c r="G19" s="14">
+        <v>647938425.50349593</v>
+      </c>
+      <c r="H19" s="14">
+        <v>409010759.14278656</v>
+      </c>
+      <c r="I19" s="14">
+        <v>564608829.7691952</v>
+      </c>
+      <c r="J19" s="14">
+        <v>563921005.13707602</v>
+      </c>
+      <c r="K19" s="14">
+        <v>327141786.18487871</v>
+      </c>
+      <c r="L19" s="14">
+        <v>493251387.84908545</v>
+      </c>
+      <c r="M19" s="14">
+        <v>311414909.38629693</v>
+      </c>
+      <c r="N19" s="14">
+        <v>301631524.01800621</v>
+      </c>
+      <c r="O19" s="14">
+        <v>207734538.80550945</v>
+      </c>
+      <c r="P19" s="14">
+        <v>311487578.80016792</v>
+      </c>
+      <c r="Q19" s="14">
+        <v>522039789.86042678</v>
+      </c>
+      <c r="R19" s="14">
+        <v>244253005.87899938</v>
+      </c>
+      <c r="S19" s="14">
+        <v>455071571.77843732</v>
+      </c>
+      <c r="T19" s="14">
+        <v>323308535.02233976</v>
+      </c>
+      <c r="U19" s="14">
+        <v>347194565.49457091</v>
+      </c>
+      <c r="V19" s="14">
+        <v>610447327.2426368</v>
+      </c>
+      <c r="W19" s="14">
+        <v>311856040.42547768</v>
+      </c>
+      <c r="X19" s="14">
+        <v>491707935.04352242</v>
+      </c>
+      <c r="Y19" s="14">
+        <v>350823905.34910131</v>
+      </c>
+      <c r="Z19" s="14">
+        <v>268971249.71056896</v>
+      </c>
+      <c r="AA19" s="14">
+        <v>492529661.91077733</v>
+      </c>
+      <c r="AB19" s="14">
+        <v>308378249.00013375</v>
+      </c>
+      <c r="AC19" s="14">
+        <v>505201602.95838773</v>
+      </c>
+      <c r="AD19" s="14">
+        <v>562461417.63607395</v>
+      </c>
+      <c r="AE19" s="14">
+        <v>659091964.86064279</v>
+      </c>
+      <c r="AF19" s="14">
+        <v>454832537.87714928</v>
+      </c>
+      <c r="AG19" s="14">
+        <v>214650075.97208297</v>
+      </c>
+      <c r="AH19" s="14">
+        <v>330184966.17132545</v>
+      </c>
+      <c r="AI19" s="14">
+        <v>153055288.87643489</v>
+      </c>
+      <c r="AJ19" s="14">
+        <v>315689544.08611357</v>
+      </c>
+      <c r="AK19" s="14">
+        <v>429164166.67439073</v>
+      </c>
+      <c r="AL19" s="14">
+        <v>255662120.90318602</v>
+      </c>
+      <c r="AM19" s="14">
+        <v>361352842.107759</v>
+      </c>
+      <c r="AN19" s="14">
+        <v>356038416.05354619</v>
+      </c>
+      <c r="AO19" s="14">
+        <v>294935943.00426137</v>
+      </c>
+      <c r="AP19" s="14">
+        <v>255742762.18248725</v>
+      </c>
+      <c r="AQ19" s="7"/>
+      <c r="AR19" s="7"/>
+      <c r="AS19" s="7"/>
+      <c r="AT19" s="7"/>
+    </row>
+    <row r="20" spans="2:46" x14ac:dyDescent="0.3">
+      <c r="B20" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="C20" s="14">
+        <v>214898011.30066893</v>
+      </c>
+      <c r="D20" s="14">
+        <v>423666094.65765154</v>
+      </c>
+      <c r="E20" s="14">
+        <v>559069996.73261976</v>
+      </c>
+      <c r="F20" s="14">
+        <v>397191990.50649184</v>
+      </c>
+      <c r="G20" s="14">
+        <v>434389766.86236644</v>
+      </c>
+      <c r="H20" s="14">
+        <v>463384227.51724088</v>
+      </c>
+      <c r="I20" s="14">
+        <v>475400085.34752083</v>
+      </c>
+      <c r="J20" s="14">
+        <v>374830318.98494107</v>
+      </c>
+      <c r="K20" s="14">
+        <v>360512240.65665102</v>
+      </c>
+      <c r="L20" s="14">
+        <v>416533892.07776266</v>
+      </c>
+      <c r="M20" s="14">
+        <v>328317237.03024983</v>
+      </c>
+      <c r="N20" s="14">
+        <v>435457051.16876143</v>
+      </c>
+      <c r="O20" s="14">
+        <v>551385286.29638076</v>
+      </c>
+      <c r="P20" s="14">
+        <v>422869456.86162466</v>
+      </c>
+      <c r="Q20" s="14">
+        <v>364209559.81617445</v>
+      </c>
+      <c r="R20" s="14">
+        <v>379373466.69386458</v>
+      </c>
+      <c r="S20" s="14">
+        <v>279141845.51547813</v>
+      </c>
+      <c r="T20" s="14">
+        <v>687914705.10731554</v>
+      </c>
+      <c r="U20" s="14">
+        <v>272704140.17576581</v>
+      </c>
+      <c r="V20" s="14">
+        <v>398961951.75829273</v>
+      </c>
+      <c r="W20" s="14">
+        <v>206683312.38013345</v>
+      </c>
+      <c r="X20" s="14">
+        <v>414987162.17056865</v>
+      </c>
+      <c r="Y20" s="14">
+        <v>368931121.93711191</v>
+      </c>
+      <c r="Z20" s="14">
+        <v>288113079.40916455</v>
+      </c>
+      <c r="AA20" s="14">
+        <v>449652019.0388248</v>
+      </c>
+      <c r="AB20" s="14">
+        <v>251345293.15233967</v>
+      </c>
+      <c r="AC20" s="14">
+        <v>502212973.05050254</v>
+      </c>
+      <c r="AD20" s="14">
+        <v>433790363.29459745</v>
+      </c>
+      <c r="AE20" s="14">
+        <v>356536662.86831206</v>
+      </c>
+      <c r="AF20" s="14">
+        <v>287960062.02577585</v>
+      </c>
+      <c r="AG20" s="14">
+        <v>275923606.6127575</v>
+      </c>
+      <c r="AH20" s="14">
+        <v>300931799.09870911</v>
+      </c>
+      <c r="AI20" s="14">
+        <v>233621355.46957704</v>
+      </c>
+      <c r="AJ20" s="15">
+        <v>414450768.71909112</v>
+      </c>
+      <c r="AK20" s="14">
+        <v>519591545.80593681</v>
+      </c>
+      <c r="AL20" s="14">
+        <v>297860832.97183752</v>
+      </c>
+      <c r="AM20" s="14">
+        <v>434186389.95240355</v>
+      </c>
+      <c r="AN20" s="14">
+        <v>479213263.19942445</v>
+      </c>
+      <c r="AO20" s="14">
+        <v>314652201.70134705</v>
+      </c>
+      <c r="AP20" s="14">
+        <v>441280515.94843221</v>
+      </c>
+      <c r="AQ20" s="7"/>
+      <c r="AR20" s="7"/>
+      <c r="AS20" s="7"/>
+      <c r="AT20" s="7"/>
+    </row>
+    <row r="21" spans="2:46" x14ac:dyDescent="0.3">
+      <c r="B21" s="13"/>
+    </row>
+    <row r="22" spans="2:46" x14ac:dyDescent="0.3">
+      <c r="B22" s="13"/>
+    </row>
+    <row r="23" spans="2:46" x14ac:dyDescent="0.3">
+      <c r="B23" s="12" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="24" spans="2:46" x14ac:dyDescent="0.3">
+      <c r="C24" t="s">
+        <v>16</v>
+      </c>
+      <c r="W24" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="25" spans="2:46" x14ac:dyDescent="0.3">
+      <c r="C25" s="2">
+        <v>1</v>
+      </c>
+      <c r="D25" s="2">
+        <v>3</v>
+      </c>
+      <c r="E25" s="2">
+        <v>4</v>
+      </c>
+      <c r="F25" s="3">
+        <v>6</v>
+      </c>
+      <c r="G25" s="2">
+        <v>7</v>
+      </c>
+      <c r="H25" s="2">
+        <v>8</v>
+      </c>
+      <c r="I25" s="2">
+        <v>9</v>
+      </c>
+      <c r="J25" s="3">
+        <v>10</v>
+      </c>
+      <c r="K25" s="2">
+        <v>11</v>
+      </c>
+      <c r="L25" s="2">
+        <v>13</v>
+      </c>
+      <c r="M25" s="2">
+        <v>15</v>
+      </c>
+      <c r="N25" s="3">
+        <v>16</v>
+      </c>
+      <c r="O25" s="2">
+        <v>18</v>
+      </c>
+      <c r="P25" s="2">
+        <v>20</v>
+      </c>
+      <c r="Q25" s="2">
+        <v>22</v>
+      </c>
+      <c r="R25" s="3">
+        <v>24</v>
+      </c>
+      <c r="S25" s="2">
+        <v>25</v>
+      </c>
+      <c r="T25" s="2">
+        <v>26</v>
+      </c>
+      <c r="U25" s="2">
+        <v>30</v>
+      </c>
+      <c r="V25" s="3">
+        <v>31</v>
+      </c>
+      <c r="W25" s="2">
+        <v>1</v>
+      </c>
+      <c r="X25" s="2">
+        <v>3</v>
+      </c>
+      <c r="Y25" s="2">
+        <v>4</v>
+      </c>
+      <c r="Z25" s="3">
+        <v>6</v>
+      </c>
+      <c r="AA25" s="2">
+        <v>7</v>
+      </c>
+      <c r="AB25" s="2">
+        <v>8</v>
+      </c>
+      <c r="AC25" s="2">
+        <v>9</v>
+      </c>
+      <c r="AD25" s="3">
+        <v>10</v>
+      </c>
+      <c r="AE25" s="2">
+        <v>11</v>
+      </c>
+      <c r="AF25" s="2">
+        <v>13</v>
+      </c>
+      <c r="AG25" s="2">
+        <v>15</v>
+      </c>
+      <c r="AH25" s="3">
+        <v>16</v>
+      </c>
+      <c r="AI25" s="2">
+        <v>18</v>
+      </c>
+      <c r="AJ25" s="2">
+        <v>20</v>
+      </c>
+      <c r="AK25" s="2">
+        <v>22</v>
+      </c>
+      <c r="AL25" s="3">
+        <v>24</v>
+      </c>
+      <c r="AM25" s="2">
+        <v>25</v>
+      </c>
+      <c r="AN25" s="2">
+        <v>26</v>
+      </c>
+      <c r="AO25" s="2">
+        <v>30</v>
+      </c>
+      <c r="AP25" s="3">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="26" spans="2:46" x14ac:dyDescent="0.3">
+      <c r="B26" t="s">
+        <v>14</v>
+      </c>
+      <c r="C26" s="14">
+        <v>804640974.41260111</v>
+      </c>
+      <c r="D26" s="14">
+        <v>558078691.46158397</v>
+      </c>
+      <c r="E26" s="14">
+        <v>353008060.87718546</v>
+      </c>
+      <c r="F26" s="14">
+        <v>319202250.87106049</v>
+      </c>
+      <c r="G26" s="14">
+        <v>643653848.23290384</v>
+      </c>
+      <c r="H26" s="14">
+        <v>439414304.7049709</v>
+      </c>
+      <c r="I26" s="14">
+        <v>615039603.26011777</v>
+      </c>
+      <c r="J26" s="14">
+        <v>610727700.22779596</v>
+      </c>
+      <c r="K26" s="14">
+        <v>350146724.08665985</v>
+      </c>
+      <c r="L26" s="14">
+        <v>533562912.5366388</v>
+      </c>
+      <c r="M26" s="14">
+        <v>339955678.05361634</v>
+      </c>
+      <c r="N26" s="14">
+        <v>328941198.54782873</v>
+      </c>
+      <c r="O26" s="14">
+        <v>219345521.60450959</v>
+      </c>
+      <c r="P26" s="14">
+        <v>338572878.77686268</v>
+      </c>
+      <c r="Q26" s="14">
+        <v>541675401.2513957</v>
+      </c>
+      <c r="R26" s="14">
+        <v>255159477.8409487</v>
+      </c>
+      <c r="S26" s="14">
+        <v>496583716.04418415</v>
+      </c>
+      <c r="T26" s="14">
+        <v>340878992.40867043</v>
+      </c>
+      <c r="U26" s="14">
+        <v>375215526.09227496</v>
+      </c>
+      <c r="V26" s="14">
+        <v>658661894.83163524</v>
+      </c>
+      <c r="W26" s="14">
+        <v>338581224.63896865</v>
+      </c>
+      <c r="X26" s="14">
+        <v>534021215.39025092</v>
+      </c>
+      <c r="Y26" s="14">
+        <v>378887498.69939959</v>
+      </c>
+      <c r="Z26" s="14">
+        <v>292733091.92494136</v>
+      </c>
+      <c r="AA26" s="14">
+        <v>531132638.17604506</v>
+      </c>
+      <c r="AB26" s="14">
+        <v>335520631.79963726</v>
+      </c>
+      <c r="AC26" s="14">
+        <v>550093819.7089963</v>
+      </c>
+      <c r="AD26" s="14">
+        <v>605182702.77742541</v>
+      </c>
+      <c r="AE26" s="14">
+        <v>717278299.39155602</v>
+      </c>
+      <c r="AF26" s="14">
+        <v>489832982.76788175</v>
+      </c>
+      <c r="AG26" s="14">
+        <v>232252924.12261975</v>
+      </c>
+      <c r="AH26" s="14">
+        <v>352009148.24736828</v>
+      </c>
+      <c r="AI26" s="14">
+        <v>165208797.41725069</v>
+      </c>
+      <c r="AJ26" s="14">
+        <v>343336795.74366367</v>
+      </c>
+      <c r="AK26" s="14">
+        <v>444670453.82702816</v>
+      </c>
+      <c r="AL26" s="14">
+        <v>267920036.64476144</v>
+      </c>
+      <c r="AM26" s="14">
+        <v>392820799.68730742</v>
+      </c>
+      <c r="AN26" s="14">
+        <v>386269012.00387782</v>
+      </c>
+      <c r="AO26" s="14">
+        <v>318786275.03503573</v>
+      </c>
+      <c r="AP26" s="14">
+        <v>267104691.86022127</v>
+      </c>
+      <c r="AQ26" s="7"/>
+      <c r="AR26" s="7"/>
+      <c r="AS26" s="7"/>
+      <c r="AT26" s="7"/>
+    </row>
+    <row r="27" spans="2:46" x14ac:dyDescent="0.3">
+      <c r="B27" t="s">
+        <v>15</v>
+      </c>
+      <c r="C27" s="14">
+        <v>231226580.18520504</v>
+      </c>
+      <c r="D27" s="14">
+        <v>457684642.89048725</v>
+      </c>
+      <c r="E27" s="14">
+        <v>607967311.58965254</v>
+      </c>
+      <c r="F27" s="14">
+        <v>431006081.5449121</v>
+      </c>
+      <c r="G27" s="14">
+        <v>447898280.91332948</v>
+      </c>
+      <c r="H27" s="14">
+        <v>505077266.00238889</v>
+      </c>
+      <c r="I27" s="14">
+        <v>517990855.99949557</v>
+      </c>
+      <c r="J27" s="14">
+        <v>405442588.99324918</v>
+      </c>
+      <c r="K27" s="14">
+        <v>389242599.64714235</v>
+      </c>
+      <c r="L27" s="14">
+        <v>449271688.22870517</v>
+      </c>
+      <c r="M27" s="14">
+        <v>357393807.69002903</v>
+      </c>
+      <c r="N27" s="14">
+        <v>474612981.34682161</v>
+      </c>
+      <c r="O27" s="14">
+        <v>599873067.91863489</v>
+      </c>
+      <c r="P27" s="14">
+        <v>458478548.23369271</v>
+      </c>
+      <c r="Q27" s="14">
+        <v>369195306.44153094</v>
+      </c>
+      <c r="R27" s="14">
+        <v>406056454.67109674</v>
+      </c>
+      <c r="S27" s="14">
+        <v>303414065.3276602</v>
+      </c>
+      <c r="T27" s="14">
+        <v>750928764.09016478</v>
+      </c>
+      <c r="U27" s="14">
+        <v>294039029.86374986</v>
+      </c>
+      <c r="V27" s="14">
+        <v>429541116.84937263</v>
+      </c>
+      <c r="W27" s="14">
+        <v>219481821.36640733</v>
+      </c>
+      <c r="X27" s="14">
+        <v>452089446.69221562</v>
+      </c>
+      <c r="Y27" s="14">
+        <v>395670673.6314767</v>
+      </c>
+      <c r="Z27" s="14">
+        <v>312792806.17045593</v>
+      </c>
+      <c r="AA27" s="14">
+        <v>480494437.3492291</v>
+      </c>
+      <c r="AB27" s="14">
+        <v>274386130.16265339</v>
+      </c>
+      <c r="AC27" s="14">
+        <v>547646554.83227563</v>
+      </c>
+      <c r="AD27" s="14">
+        <v>470638006.42611706</v>
+      </c>
+      <c r="AE27" s="14">
+        <v>380765734.66973066</v>
+      </c>
+      <c r="AF27" s="14">
+        <v>312208119.77422369</v>
+      </c>
+      <c r="AG27" s="14">
+        <v>301206275.21211773</v>
+      </c>
+      <c r="AH27" s="14">
+        <v>323428629.73202848</v>
+      </c>
+      <c r="AI27" s="14">
+        <v>252057013.70192561</v>
+      </c>
+      <c r="AJ27" s="15">
+        <v>451457259.36730492</v>
+      </c>
+      <c r="AK27" s="14">
+        <v>563477987.88546789</v>
+      </c>
+      <c r="AL27" s="14">
+        <v>311249431.22501284</v>
+      </c>
+      <c r="AM27" s="14">
+        <v>471540276.04321176</v>
+      </c>
+      <c r="AN27" s="14">
+        <v>522061684.17020947</v>
+      </c>
+      <c r="AO27" s="14">
+        <v>339777957.49942833</v>
+      </c>
+      <c r="AP27" s="14">
+        <v>481165795.80438107</v>
+      </c>
+      <c r="AQ27" s="7"/>
+      <c r="AR27" s="7"/>
+      <c r="AS27" s="7"/>
+      <c r="AT27" s="7"/>
+    </row>
+  </sheetData>
+  <conditionalFormatting sqref="B1">
+    <cfRule type="colorScale" priority="5">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B8">
+    <cfRule type="colorScale" priority="4">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B23">
+    <cfRule type="colorScale" priority="2">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B16">
+    <cfRule type="colorScale" priority="1">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>